<commit_message>
Finalize main board and bom
</commit_message>
<xml_diff>
--- a/Electrical/MainBoard/bom/digikeyV0.3.xlsx
+++ b/Electrical/MainBoard/bom/digikeyV0.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satom\Desktop\Robot\Electrical\MainBoard\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFF38B6-AE60-40DC-BF3C-ADD289E85799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEAA69C-4A0C-496B-9118-3B4E8A82A59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7725" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="228">
   <si>
     <t>References</t>
   </si>
@@ -165,9 +165,6 @@
     <t>RMCF0805ZT0R00CT-ND</t>
   </si>
   <si>
-    <t>R2, R12, R13, R14</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -330,21 +327,12 @@
     <t>296-29575-1-ND</t>
   </si>
   <si>
-    <t>U11, U12</t>
-  </si>
-  <si>
-    <t>Quad_Encoder_Motor</t>
-  </si>
-  <si>
     <t>Molex_KK-254_AE-6410-06A_1x06_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>Molex</t>
   </si>
   <si>
-    <t>WM4115-ND</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -408,9 +396,6 @@
     <t>36-4628-ND</t>
   </si>
   <si>
-    <t>SW4, SW5, SW6</t>
-  </si>
-  <si>
     <t>User_Button</t>
   </si>
   <si>
@@ -525,12 +510,6 @@
     <t>S1111EC-06-ND</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>3.3V Supply</t>
-  </si>
-  <si>
     <t>PinHeader_2x05_P2.54mm_Vertical</t>
   </si>
   <si>
@@ -543,18 +522,6 @@
     <t>2057-PH2-10-UA-ND</t>
   </si>
   <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>5V Supply</t>
-  </si>
-  <si>
-    <t>J20</t>
-  </si>
-  <si>
-    <t>Conn_01x06</t>
-  </si>
-  <si>
     <t>J26</t>
   </si>
   <si>
@@ -564,9 +531,6 @@
     <t>PinHeader_2x04_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C19, C22, C23, C24, C27, C28, C30, C31, C32, C36</t>
-  </si>
-  <si>
     <t>KEMET</t>
   </si>
   <si>
@@ -591,18 +555,6 @@
     <t>3147-B1701UD--20D000414U1930CT-ND</t>
   </si>
   <si>
-    <t>J24</t>
-  </si>
-  <si>
-    <t>Conn_01x04</t>
-  </si>
-  <si>
-    <t>CONN_22-23-2041_MOL</t>
-  </si>
-  <si>
-    <t>WM4202-ND</t>
-  </si>
-  <si>
     <t>METZ CONNECT USA Inc.</t>
   </si>
   <si>
@@ -633,12 +585,6 @@
     <t>900-0022013037-ND</t>
   </si>
   <si>
-    <t>4 Pin Female</t>
-  </si>
-  <si>
-    <t>WM2002-ND</t>
-  </si>
-  <si>
     <t>Crimps</t>
   </si>
   <si>
@@ -661,6 +607,108 @@
   </si>
   <si>
     <t>WM20948CT-ND</t>
+  </si>
+  <si>
+    <t>Littlefuse Inc.</t>
+  </si>
+  <si>
+    <t>6 Pin Female</t>
+  </si>
+  <si>
+    <t>WM2015-ND</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C19, C22, C23, C24, C27, C28, C30, C31, C32, C35, C36</t>
+  </si>
+  <si>
+    <t>J20, U11, U12</t>
+  </si>
+  <si>
+    <t>Conn_01x06, Quad_Encoder_Motor</t>
+  </si>
+  <si>
+    <t>WM4204-ND</t>
+  </si>
+  <si>
+    <t>J2, J3</t>
+  </si>
+  <si>
+    <t>3.3V Supply, 5V Supply</t>
+  </si>
+  <si>
+    <t>J17</t>
+  </si>
+  <si>
+    <t>MEM2061-01-188-00-A</t>
+  </si>
+  <si>
+    <t>MEM2061-01-188-00-A_GCT</t>
+  </si>
+  <si>
+    <t>GCT</t>
+  </si>
+  <si>
+    <t>2073-MEM2061-01-188-00-ACT-ND</t>
+  </si>
+  <si>
+    <t>R2, R14</t>
+  </si>
+  <si>
+    <t>SW6</t>
+  </si>
+  <si>
+    <t>F1725-ND</t>
+  </si>
+  <si>
+    <t>0217005.MXP</t>
+  </si>
+  <si>
+    <t>100 nF</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t>BMI323</t>
+  </si>
+  <si>
+    <t>BMI323_BOS-M</t>
+  </si>
+  <si>
+    <t>IMU ACCEL/GYRO I2C/SPI 14LGA</t>
+  </si>
+  <si>
+    <t>Bosch</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>828-BMI323CT-ND</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Pin</t>
+  </si>
+  <si>
+    <t>PinSocket_1x04_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 4POS 2.54MM</t>
+  </si>
+  <si>
+    <t>10129378-904001BLF</t>
+  </si>
+  <si>
+    <t>10129378-904001BLF-ND</t>
+  </si>
+  <si>
+    <t>IMU-C1, C2</t>
+  </si>
+  <si>
+    <t>IMU-U1</t>
+  </si>
+  <si>
+    <t>IMU-J1, J2</t>
   </si>
 </sst>
 </file>
@@ -692,7 +740,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -700,13 +748,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1027,7 +1086,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1048,7 +1107,7 @@
         <v>13</v>
       </c>
       <c r="H2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1114,16 +1173,16 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -1235,25 +1294,25 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H10">
         <v>4</v>
@@ -1261,36 +1320,36 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>208</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -1299,24 +1358,24 @@
         <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
         <v>60</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
@@ -1325,13 +1384,13 @@
         <v>39</v>
       </c>
       <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
         <v>62</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>63</v>
       </c>
       <c r="H13">
         <v>2</v>
@@ -1339,10 +1398,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
         <v>64</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -1351,13 +1410,13 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
         <v>66</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" t="s">
-        <v>67</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -1365,10 +1424,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
         <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -1377,13 +1436,13 @@
         <v>39</v>
       </c>
       <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
         <v>70</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>71</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -1391,25 +1450,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
         <v>72</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
         <v>73</v>
       </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
         <v>74</v>
-      </c>
-      <c r="F16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" t="s">
-        <v>75</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -1417,25 +1476,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
         <v>76</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>77</v>
       </c>
-      <c r="C17" t="s">
-        <v>78</v>
-      </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E17" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="H17">
         <v>6</v>
@@ -1443,25 +1502,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
         <v>77</v>
       </c>
-      <c r="C18" t="s">
-        <v>78</v>
-      </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E18" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="H18">
         <v>3</v>
@@ -1469,25 +1528,25 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>82</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>83</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
         <v>84</v>
-      </c>
-      <c r="F19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" t="s">
-        <v>85</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1495,25 +1554,25 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" t="s">
         <v>86</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>87</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>88</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
         <v>89</v>
-      </c>
-      <c r="E20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" t="s">
-        <v>90</v>
       </c>
       <c r="H20">
         <v>4</v>
@@ -1521,25 +1580,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
         <v>91</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>92</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>93</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
         <v>94</v>
-      </c>
-      <c r="E21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" t="s">
-        <v>95</v>
       </c>
       <c r="H21">
         <v>2</v>
@@ -1547,25 +1606,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
         <v>96</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>97</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>98</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
         <v>99</v>
-      </c>
-      <c r="E22" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" t="s">
-        <v>100</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -1573,51 +1632,51 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" t="s">
         <v>103</v>
       </c>
-      <c r="D23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23">
-        <v>22272061</v>
-      </c>
       <c r="F23" t="s">
         <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1625,25 +1684,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1651,25 +1710,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+      <c r="E26">
+        <v>4628</v>
       </c>
       <c r="F26" t="s">
         <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1677,25 +1736,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B27" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
-      </c>
-      <c r="E27">
-        <v>4628</v>
+        <v>129</v>
+      </c>
+      <c r="E27" t="s">
+        <v>130</v>
       </c>
       <c r="F27" t="s">
         <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1703,51 +1762,51 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28">
-        <v>22232021</v>
+        <v>135</v>
+      </c>
+      <c r="E28" t="s">
+        <v>136</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="H28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C29" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D29" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E29" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="F29" t="s">
         <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1755,25 +1814,25 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>209</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D30" t="s">
-        <v>140</v>
-      </c>
-      <c r="E30" t="s">
-        <v>141</v>
+        <v>101</v>
+      </c>
+      <c r="E30">
+        <v>22232021</v>
       </c>
       <c r="F30" t="s">
         <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1781,396 +1840,455 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>198</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>199</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
-      </c>
-      <c r="E31" t="s">
-        <v>147</v>
+        <v>101</v>
+      </c>
+      <c r="E31">
+        <v>22232061</v>
       </c>
       <c r="F31" t="s">
         <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>148</v>
+        <v>200</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="B32" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="C32" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="D32" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="E32" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="H32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B33" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C33" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33">
-        <v>1017514</v>
+        <v>147</v>
+      </c>
+      <c r="E33" t="s">
+        <v>148</v>
       </c>
       <c r="F33" t="s">
         <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" t="s">
+        <v>153</v>
+      </c>
+      <c r="E34">
+        <v>1017514</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>154</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" t="s">
+        <v>159</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
         <v>160</v>
-      </c>
-      <c r="B34" t="s">
-        <v>161</v>
-      </c>
-      <c r="C34" t="s">
-        <v>162</v>
-      </c>
-      <c r="D34" t="s">
-        <v>163</v>
-      </c>
-      <c r="E34" t="s">
-        <v>164</v>
-      </c>
-      <c r="F34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" t="s">
-        <v>165</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>166</v>
-      </c>
-      <c r="B35" t="s">
-        <v>167</v>
-      </c>
-      <c r="C35" t="s">
-        <v>168</v>
-      </c>
-      <c r="D35" t="s">
-        <v>169</v>
-      </c>
-      <c r="E35" t="s">
-        <v>170</v>
-      </c>
-      <c r="F35" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" t="s">
-        <v>171</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="B36" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="D36" t="s">
-        <v>169</v>
+        <v>206</v>
       </c>
       <c r="E36" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37">
-        <v>22272061</v>
+        <v>176</v>
+      </c>
+      <c r="E37" t="s">
+        <v>177</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>105</v>
+        <v>178</v>
       </c>
       <c r="H37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>188</v>
-      </c>
-      <c r="B38" t="s">
-        <v>189</v>
-      </c>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D38" t="s">
-        <v>104</v>
-      </c>
-      <c r="E38">
-        <v>22232041</v>
+        <v>141</v>
+      </c>
+      <c r="E38" t="s">
+        <v>180</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>176</v>
-      </c>
-      <c r="B39" t="s">
-        <v>177</v>
-      </c>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C39" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D39" t="s">
-        <v>192</v>
-      </c>
-      <c r="E39" t="s">
-        <v>193</v>
+        <v>101</v>
+      </c>
+      <c r="E39">
+        <v>22013027</v>
       </c>
       <c r="F39" t="s">
         <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C41" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C40" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40">
+        <v>22013037</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="s">
+        <v>185</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C41" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D41" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D41" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="2">
+        <v>22012067</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F41" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" t="s">
-        <v>197</v>
-      </c>
-      <c r="H41">
+      <c r="H41" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="D42" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E42">
-        <v>22013027</v>
+        <v>8650804</v>
       </c>
       <c r="F42" t="s">
         <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="H42">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C43" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D43" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E43">
-        <v>22013037</v>
+        <v>26604040</v>
       </c>
       <c r="F43" t="s">
         <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C44" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D44" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E44">
-        <v>22013047</v>
+        <v>9508041</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="H44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C45" t="s">
+        <v>192</v>
+      </c>
+      <c r="D45" t="s">
+        <v>101</v>
+      </c>
+      <c r="E45">
+        <v>8500008</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
+        <v>193</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H46" s="3">
+        <v>1</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>225</v>
+      </c>
+      <c r="B47" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>213</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C45" t="s">
-        <v>204</v>
-      </c>
-      <c r="D45" t="s">
-        <v>104</v>
-      </c>
-      <c r="E45">
-        <v>8650804</v>
-      </c>
-      <c r="F45" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" t="s">
-        <v>205</v>
-      </c>
-      <c r="H45">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C46" t="s">
-        <v>206</v>
-      </c>
-      <c r="D46" t="s">
-        <v>104</v>
-      </c>
-      <c r="E46">
-        <v>26604040</v>
-      </c>
-      <c r="F46" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" t="s">
-        <v>207</v>
-      </c>
-      <c r="H46">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>226</v>
+      </c>
+      <c r="B48" t="s">
+        <v>214</v>
+      </c>
+      <c r="C48" t="s">
+        <v>215</v>
+      </c>
+      <c r="D48" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" t="s">
+        <v>217</v>
+      </c>
+      <c r="F48" t="s">
+        <v>214</v>
+      </c>
+      <c r="G48" t="s">
+        <v>218</v>
+      </c>
+      <c r="H48" t="s">
+        <v>219</v>
+      </c>
+      <c r="I48">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C47" t="s">
-        <v>208</v>
-      </c>
-      <c r="D47" t="s">
-        <v>104</v>
-      </c>
-      <c r="E47">
-        <v>9508041</v>
-      </c>
-      <c r="F47" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" t="s">
-        <v>209</v>
-      </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C48" t="s">
-        <v>210</v>
-      </c>
-      <c r="D48" t="s">
-        <v>104</v>
-      </c>
-      <c r="E48">
-        <v>8500008</v>
-      </c>
-      <c r="F48" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" t="s">
-        <v>211</v>
-      </c>
-      <c r="H48">
-        <v>4</v>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>227</v>
+      </c>
+      <c r="B49" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" t="s">
+        <v>221</v>
+      </c>
+      <c r="D49" t="s">
+        <v>222</v>
+      </c>
+      <c r="E49" t="s">
+        <v>147</v>
+      </c>
+      <c r="F49" t="s">
+        <v>223</v>
+      </c>
+      <c r="G49" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s">
+        <v>224</v>
+      </c>
+      <c r="I49">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 3 pin male to BOM
</commit_message>
<xml_diff>
--- a/Electrical/MainBoard/bom/digikeyV0.3.xlsx
+++ b/Electrical/MainBoard/bom/digikeyV0.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satom\Desktop\Robot\Electrical\MainBoard\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEAA69C-4A0C-496B-9118-3B4E8A82A59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A543787-9FD3-4F42-A928-98B4CD4467FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="228">
   <si>
     <t>References</t>
   </si>
@@ -663,9 +663,6 @@
     <t>0217005.MXP</t>
   </si>
   <si>
-    <t>100 nF</t>
-  </si>
-  <si>
     <t>CAP CER 0.1UF 50V X7R 0805</t>
   </si>
   <si>
@@ -687,9 +684,6 @@
     <t>828-BMI323CT-ND</t>
   </si>
   <si>
-    <t>Conn_01x04_Pin</t>
-  </si>
-  <si>
     <t>PinSocket_1x04_P2.54mm_Vertical</t>
   </si>
   <si>
@@ -709,6 +703,12 @@
   </si>
   <si>
     <t>IMU-J1, J2</t>
+  </si>
+  <si>
+    <t>3 Pin Male</t>
+  </si>
+  <si>
+    <t>WM4201-ND</t>
   </si>
 </sst>
 </file>
@@ -761,10 +761,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1046,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2081,80 +2080,80 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C41" s="2" t="s">
+      <c r="C41" t="s">
         <v>195</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41">
         <v>22012067</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" t="s">
         <v>196</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="D42" t="s">
         <v>101</v>
       </c>
       <c r="E42">
-        <v>8650804</v>
+        <v>22232031</v>
       </c>
       <c r="F42" t="s">
         <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="H42">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D43" t="s">
         <v>101</v>
       </c>
       <c r="E43">
-        <v>26604040</v>
+        <v>8650804</v>
       </c>
       <c r="F43" t="s">
         <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C44" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D44" t="s">
         <v>101</v>
       </c>
       <c r="E44">
-        <v>9508041</v>
+        <v>26604040</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -2162,132 +2161,143 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C45" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D45" t="s">
         <v>101</v>
       </c>
       <c r="E45">
+        <v>9508041</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
+        <v>191</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C46" t="s">
+        <v>192</v>
+      </c>
+      <c r="D46" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46">
         <v>8500008</v>
       </c>
-      <c r="F45" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" t="s">
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
         <v>193</v>
       </c>
-      <c r="H45">
+      <c r="H46">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E47" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="3" t="s">
+      <c r="F47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H47" s="2">
         <v>1</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="s">
-        <v>225</v>
-      </c>
-      <c r="B47" t="s">
-        <v>212</v>
-      </c>
-      <c r="C47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" t="s">
-        <v>213</v>
-      </c>
-      <c r="E47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" t="s">
-        <v>13</v>
-      </c>
-      <c r="I47">
-        <v>2</v>
-      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>212</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>224</v>
+      </c>
+      <c r="B49" t="s">
         <v>214</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>215</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>216</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
+        <v>213</v>
+      </c>
+      <c r="F49" t="s">
         <v>217</v>
       </c>
-      <c r="F48" t="s">
-        <v>214</v>
-      </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>218</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>225</v>
+      </c>
+      <c r="B50" t="s">
         <v>219</v>
       </c>
-      <c r="I48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" t="s">
-        <v>227</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C50" t="s">
         <v>220</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D50" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" t="s">
         <v>221</v>
       </c>
-      <c r="D49" t="s">
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
         <v>222</v>
       </c>
-      <c r="E49" t="s">
-        <v>147</v>
-      </c>
-      <c r="F49" t="s">
-        <v>223</v>
-      </c>
-      <c r="G49" t="s">
-        <v>12</v>
-      </c>
-      <c r="H49" t="s">
-        <v>224</v>
-      </c>
-      <c r="I49">
+      <c r="H50">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the status LED to common anode
</commit_message>
<xml_diff>
--- a/Electrical/MainBoard/bom/digikeyV0.3.xlsx
+++ b/Electrical/MainBoard/bom/digikeyV0.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satom\Desktop\Robot\Electrical\MainBoard\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A543787-9FD3-4F42-A928-98B4CD4467FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A457613-B675-4F13-B855-BE36ABE14A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,12 +276,6 @@
     <t>Kingbright</t>
   </si>
   <si>
-    <t>WP115WGYW</t>
-  </si>
-  <si>
-    <t>754-1864-ND</t>
-  </si>
-  <si>
     <t>U5, U6, U7, U8</t>
   </si>
   <si>
@@ -709,6 +703,12 @@
   </si>
   <si>
     <t>WM4201-ND</t>
+  </si>
+  <si>
+    <t>WP59EGW/CA</t>
+  </si>
+  <si>
+    <t>754-2191-ND</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1172,16 +1172,16 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
         <v>168</v>
-      </c>
-      <c r="E5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>170</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B12" t="s">
         <v>46</v>
@@ -1484,16 +1484,16 @@
         <v>77</v>
       </c>
       <c r="D17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
         <v>171</v>
-      </c>
-      <c r="E17" t="s">
-        <v>172</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" t="s">
-        <v>173</v>
       </c>
       <c r="H17">
         <v>6</v>
@@ -1510,16 +1510,16 @@
         <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H18">
         <v>3</v>
@@ -1539,13 +1539,13 @@
         <v>82</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>226</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>227</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1553,25 +1553,25 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
         <v>85</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>86</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
         <v>87</v>
-      </c>
-      <c r="D20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" t="s">
-        <v>89</v>
       </c>
       <c r="H20">
         <v>4</v>
@@ -1579,25 +1579,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
         <v>90</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>91</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
         <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" t="s">
-        <v>94</v>
       </c>
       <c r="H21">
         <v>2</v>
@@ -1605,25 +1605,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
         <v>95</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>96</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
         <v>97</v>
-      </c>
-      <c r="D22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" t="s">
-        <v>99</v>
       </c>
       <c r="H22">
         <v>2</v>
@@ -1631,25 +1631,25 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" t="s">
         <v>102</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>103</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
         <v>104</v>
-      </c>
-      <c r="D23" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" t="s">
-        <v>106</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1657,25 +1657,25 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
         <v>107</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
         <v>108</v>
       </c>
-      <c r="C24" t="s">
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
         <v>109</v>
-      </c>
-      <c r="D24" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" t="s">
-        <v>110</v>
-      </c>
-      <c r="F24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" t="s">
-        <v>111</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1683,25 +1683,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" t="s">
         <v>112</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>113</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>114</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
         <v>115</v>
-      </c>
-      <c r="E25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" t="s">
-        <v>117</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1709,16 +1709,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
         <v>118</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>119</v>
-      </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" t="s">
-        <v>121</v>
       </c>
       <c r="E26">
         <v>4628</v>
@@ -1727,7 +1727,7 @@
         <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1735,25 +1735,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" t="s">
         <v>126</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>127</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>128</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
         <v>129</v>
-      </c>
-      <c r="E27" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" t="s">
-        <v>131</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1761,25 +1761,25 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" t="s">
         <v>132</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>133</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>134</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
         <v>135</v>
-      </c>
-      <c r="E28" t="s">
-        <v>136</v>
-      </c>
-      <c r="F28" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" t="s">
-        <v>137</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -1787,25 +1787,25 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" t="s">
         <v>138</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>139</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>140</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
         <v>141</v>
-      </c>
-      <c r="E29" t="s">
-        <v>142</v>
-      </c>
-      <c r="F29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" t="s">
-        <v>143</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1813,16 +1813,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E30">
         <v>22232021</v>
@@ -1831,7 +1831,7 @@
         <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1839,16 +1839,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E31">
         <v>22232061</v>
@@ -1857,7 +1857,7 @@
         <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H31">
         <v>3</v>
@@ -1865,25 +1865,25 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D32" t="s">
+        <v>160</v>
+      </c>
+      <c r="E32" t="s">
         <v>161</v>
       </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
         <v>162</v>
-      </c>
-      <c r="E32" t="s">
-        <v>163</v>
-      </c>
-      <c r="F32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" t="s">
-        <v>164</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -1891,25 +1891,25 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
         <v>144</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>145</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>146</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
         <v>147</v>
-      </c>
-      <c r="E33" t="s">
-        <v>148</v>
-      </c>
-      <c r="F33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" t="s">
-        <v>149</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -1917,16 +1917,16 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" t="s">
         <v>150</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>151</v>
-      </c>
-      <c r="C34" t="s">
-        <v>152</v>
-      </c>
-      <c r="D34" t="s">
-        <v>153</v>
       </c>
       <c r="E34">
         <v>1017514</v>
@@ -1935,7 +1935,7 @@
         <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H34">
         <v>2</v>
@@ -1943,25 +1943,25 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" t="s">
         <v>155</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>156</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
         <v>157</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
         <v>158</v>
-      </c>
-      <c r="E35" t="s">
-        <v>159</v>
-      </c>
-      <c r="F35" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" t="s">
-        <v>160</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -1969,25 +1969,25 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" t="s">
         <v>203</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>204</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
+        <v>202</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
         <v>205</v>
-      </c>
-      <c r="D36" t="s">
-        <v>206</v>
-      </c>
-      <c r="E36" t="s">
-        <v>204</v>
-      </c>
-      <c r="F36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" t="s">
-        <v>207</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -1995,25 +1995,25 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" t="s">
         <v>165</v>
       </c>
-      <c r="B37" t="s">
-        <v>166</v>
-      </c>
-      <c r="C37" t="s">
-        <v>167</v>
-      </c>
       <c r="D37" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" t="s">
         <v>176</v>
-      </c>
-      <c r="E37" t="s">
-        <v>177</v>
-      </c>
-      <c r="F37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" t="s">
-        <v>178</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -2021,19 +2021,19 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" t="s">
+        <v>177</v>
+      </c>
+      <c r="D38" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" t="s">
+        <v>178</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
         <v>179</v>
-      </c>
-      <c r="D38" t="s">
-        <v>141</v>
-      </c>
-      <c r="E38" t="s">
-        <v>180</v>
-      </c>
-      <c r="F38" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" t="s">
-        <v>181</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -2041,10 +2041,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E39">
         <v>22013027</v>
@@ -2053,7 +2053,7 @@
         <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -2061,10 +2061,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E40">
         <v>22013037</v>
@@ -2073,7 +2073,7 @@
         <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -2081,10 +2081,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E41">
         <v>22012067</v>
@@ -2093,7 +2093,7 @@
         <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H41">
         <v>3</v>
@@ -2101,10 +2101,10 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E42">
         <v>22232031</v>
@@ -2113,7 +2113,7 @@
         <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -2121,10 +2121,10 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C43" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E43">
         <v>8650804</v>
@@ -2133,7 +2133,7 @@
         <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H43">
         <v>30</v>
@@ -2141,10 +2141,10 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C44" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E44">
         <v>26604040</v>
@@ -2153,7 +2153,7 @@
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -2161,10 +2161,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D45" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E45">
         <v>9508041</v>
@@ -2173,7 +2173,7 @@
         <v>12</v>
       </c>
       <c r="G45" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -2181,10 +2181,10 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C46" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E46">
         <v>8500008</v>
@@ -2193,7 +2193,7 @@
         <v>12</v>
       </c>
       <c r="G46" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H46">
         <v>5</v>
@@ -2203,19 +2203,19 @@
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H47" s="2">
         <v>1</v>
@@ -2225,13 +2225,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D48" t="s">
         <v>10</v>
@@ -2251,25 +2251,25 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B49" t="s">
+        <v>212</v>
+      </c>
+      <c r="C49" t="s">
+        <v>213</v>
+      </c>
+      <c r="D49" t="s">
         <v>214</v>
       </c>
-      <c r="C49" t="s">
+      <c r="E49" t="s">
+        <v>211</v>
+      </c>
+      <c r="F49" t="s">
         <v>215</v>
       </c>
-      <c r="D49" t="s">
+      <c r="G49" t="s">
         <v>216</v>
-      </c>
-      <c r="E49" t="s">
-        <v>213</v>
-      </c>
-      <c r="F49" t="s">
-        <v>217</v>
-      </c>
-      <c r="G49" t="s">
-        <v>218</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -2277,25 +2277,25 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B50" t="s">
+        <v>217</v>
+      </c>
+      <c r="C50" t="s">
+        <v>218</v>
+      </c>
+      <c r="D50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" t="s">
         <v>219</v>
       </c>
-      <c r="C50" t="s">
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
         <v>220</v>
-      </c>
-      <c r="D50" t="s">
-        <v>147</v>
-      </c>
-      <c r="E50" t="s">
-        <v>221</v>
-      </c>
-      <c r="F50" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" t="s">
-        <v>222</v>
       </c>
       <c r="H50">
         <v>2</v>

</xml_diff>